<commit_message>
New code & new reads of non-R PALs
</commit_message>
<xml_diff>
--- a/new_reads/reads.xlsx
+++ b/new_reads/reads.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\PalAnalyzer\new_reads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F09966-3054-4518-A104-170874C28FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBD4A64-8E13-4528-8F20-D42A5EDA4333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="55">
   <si>
     <t>Ref</t>
   </si>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>10L8</t>
-  </si>
-  <si>
-    <t>tri-state?</t>
   </si>
   <si>
     <t>No</t>
@@ -637,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,7 +668,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>5</v>
@@ -680,7 +677,7 @@
         <v>6</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H1" s="14" t="s">
         <v>7</v>
@@ -694,49 +691,49 @@
         <v>3</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" t="s">
-        <v>35</v>
-      </c>
       <c r="I2" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J2" s="14"/>
       <c r="K2" s="14" t="s">
         <v>3</v>
       </c>
       <c r="R2" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>11</v>
@@ -755,7 +752,7 @@
         <v>8</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S3" s="2">
         <v>1</v>
@@ -773,22 +770,22 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
         <v>49</v>
       </c>
-      <c r="D4" t="s">
-        <v>50</v>
-      </c>
       <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
         <v>34</v>
-      </c>
-      <c r="F4" t="s">
-        <v>35</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>11</v>
@@ -835,13 +832,13 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>11</v>
@@ -888,13 +885,13 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
         <v>37</v>
       </c>
-      <c r="B6" t="s">
-        <v>38</v>
-      </c>
       <c r="I6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>11</v>
@@ -933,12 +930,12 @@
         <v>17</v>
       </c>
       <c r="W6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="I7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>11</v>
@@ -977,12 +974,12 @@
         <v>16</v>
       </c>
       <c r="W7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="I8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>11</v>
@@ -1021,7 +1018,7 @@
         <v>15</v>
       </c>
       <c r="W8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
@@ -1062,7 +1059,7 @@
         <v>14</v>
       </c>
       <c r="W9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
@@ -1185,7 +1182,7 @@
         <v>11</v>
       </c>
       <c r="W12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.3">
@@ -1230,11 +1227,8 @@
       <c r="P16" t="s">
         <v>9</v>
       </c>
-      <c r="Q16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="11:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="11:16" x14ac:dyDescent="0.3">
       <c r="K17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1253,11 +1247,8 @@
       <c r="P17" t="s">
         <v>9</v>
       </c>
-      <c r="Q17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="11:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="11:16" x14ac:dyDescent="0.3">
       <c r="K18" s="1" t="s">
         <v>11</v>
       </c>
@@ -1276,11 +1267,8 @@
       <c r="P18" t="s">
         <v>9</v>
       </c>
-      <c r="Q18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="11:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="11:16" x14ac:dyDescent="0.3">
       <c r="K19" s="1" t="s">
         <v>11</v>
       </c>
@@ -1299,11 +1287,8 @@
       <c r="P19" t="s">
         <v>9</v>
       </c>
-      <c r="Q19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="11:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="11:16" x14ac:dyDescent="0.3">
       <c r="K20" s="1" t="s">
         <v>11</v>
       </c>
@@ -1322,11 +1307,8 @@
       <c r="P20" t="s">
         <v>9</v>
       </c>
-      <c r="Q20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="11:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="11:16" x14ac:dyDescent="0.3">
       <c r="K21" s="1" t="s">
         <v>11</v>
       </c>
@@ -1345,11 +1327,8 @@
       <c r="P21" t="s">
         <v>9</v>
       </c>
-      <c r="Q21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="11:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="11:16" x14ac:dyDescent="0.3">
       <c r="K22" s="1" t="s">
         <v>11</v>
       </c>
@@ -1368,11 +1347,8 @@
       <c r="P22" t="s">
         <v>9</v>
       </c>
-      <c r="Q22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="11:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="11:16" x14ac:dyDescent="0.3">
       <c r="K23" s="1" t="s">
         <v>11</v>
       </c>
@@ -1391,11 +1367,8 @@
       <c r="P23" t="s">
         <v>9</v>
       </c>
-      <c r="Q23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="11:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="11:16" x14ac:dyDescent="0.3">
       <c r="K24" s="1" t="s">
         <v>12</v>
       </c>

</xml_diff>